<commit_message>
changed uRect to uCARD
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bengrollpmt/Documents/own_projects/upython-uxui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D18CC5-56E5-494B-BFF6-574AF059BDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A0891E-D4A3-DC44-BCF8-4EAC514AA6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{2951F315-3064-1742-B71F-ACC6776DC761}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{2951F315-3064-1742-B71F-ACC6776DC761}"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets Properties" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Height</t>
   </si>
   <si>
-    <t>uRECT</t>
-  </si>
-  <si>
     <t>uDISPLAY</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Markiert wie stark gerundet die Ecken sind, 0 = garnicht</t>
+  </si>
+  <si>
+    <t>uCARD</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,13 +540,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -558,22 +558,22 @@
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5">
         <v>880</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -585,16 +585,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5">
         <v>528</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -602,22 +602,22 @@
     </row>
     <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -625,16 +625,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -642,72 +642,72 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed BoundaryControl, entered propmod
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bengrollpmt/Documents/own_projects/upython-uxui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A0891E-D4A3-DC44-BCF8-4EAC514AA6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D278372C-D96B-8B4D-8A42-88E39B7DE65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{2951F315-3064-1742-B71F-ACC6776DC761}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>Widget</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>uCARD</t>
+  </si>
+  <si>
+    <t>filled</t>
+  </si>
+  <si>
+    <t>fill_highlight</t>
+  </si>
+  <si>
+    <t>IN =&gt; True</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Gibt an ob die Fläche des Rechtecks gefüllt werden soll</t>
   </si>
 </sst>
 </file>
@@ -517,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CB94A5-C524-8349-85A7-31424A3D5834}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,6 +725,37 @@
         <v>31</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Continue unodes.py ln 129
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bengrollpmt/Documents/own_projects/upython-uxui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D278372C-D96B-8B4D-8A42-88E39B7DE65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55411570-611E-5544-8870-3B9F587F8E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{2951F315-3064-1742-B71F-ACC6776DC761}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Widget</t>
   </si>
@@ -148,6 +148,42 @@
   </si>
   <si>
     <t>Gibt an ob die Fläche des Rechtecks gefüllt werden soll</t>
+  </si>
+  <si>
+    <t>modX</t>
+  </si>
+  <si>
+    <t>modY</t>
+  </si>
+  <si>
+    <t>modXvalue</t>
+  </si>
+  <si>
+    <t>modYvalue</t>
+  </si>
+  <si>
+    <t>alignX</t>
+  </si>
+  <si>
+    <t>alignY</t>
+  </si>
+  <si>
+    <t>IN =&gt; 100</t>
+  </si>
+  <si>
+    <t>IN =&gt; align.center</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>align.center</t>
+  </si>
+  <si>
+    <t>align.end</t>
+  </si>
+  <si>
+    <t>uPBOX</t>
   </si>
 </sst>
 </file>
@@ -532,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CB94A5-C524-8349-85A7-31424A3D5834}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,6 +792,90 @@
         <v>20</v>
       </c>
     </row>
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>